<commit_message>
Możliwość wczytywania pola typu data
</commit_message>
<xml_diff>
--- a/src/test/resources/testfiles/b2b.xlsx
+++ b/src/test/resources/testfiles/b2b.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>idx</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>Piotr</t>
+  </si>
+  <si>
+    <t>Data podpisania kontraktu</t>
+  </si>
+  <si>
+    <t>18-10-2015</t>
+  </si>
+  <si>
+    <t>25-08-2015</t>
+  </si>
+  <si>
+    <t>06-06-2016</t>
   </si>
 </sst>
 </file>
@@ -381,19 +393,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,8 +416,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -414,8 +430,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -425,8 +444,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -435,6 +457,9 @@
       </c>
       <c r="C4" t="s">
         <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>